<commit_message>
revamped Flipkart PO tool. Needs testing
</commit_message>
<xml_diff>
--- a/Database/AXOR FSN.xlsx
+++ b/Database/AXOR FSN.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB357D56-2273-40EC-94B6-47FC805CF286}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D626E606-F85B-4D6C-848B-2C84C07A8663}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t>Model Name</t>
   </si>
@@ -325,9 +325,6 @@
   </si>
   <si>
     <t>MRP</t>
-  </si>
-  <si>
-    <t>PO to be released</t>
   </si>
 </sst>
 </file>
@@ -785,20 +782,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -808,11 +804,8 @@
       <c r="C1" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -822,11 +815,8 @@
       <c r="C2" s="4">
         <v>4994</v>
       </c>
-      <c r="D2" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -836,11 +826,8 @@
       <c r="C3" s="4">
         <v>4994</v>
       </c>
-      <c r="D3" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -850,11 +837,8 @@
       <c r="C4" s="4">
         <v>4994</v>
       </c>
-      <c r="D4" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -864,11 +848,8 @@
       <c r="C5" s="4">
         <v>4994</v>
       </c>
-      <c r="D5" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -878,11 +859,8 @@
       <c r="C6" s="4">
         <v>4994</v>
       </c>
-      <c r="D6" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -892,11 +870,8 @@
       <c r="C7" s="4">
         <v>4994</v>
       </c>
-      <c r="D7" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -906,11 +881,8 @@
       <c r="C8" s="4">
         <v>4994</v>
       </c>
-      <c r="D8" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -920,11 +892,8 @@
       <c r="C9" s="4">
         <v>4994</v>
       </c>
-      <c r="D9" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -934,11 +903,8 @@
       <c r="C10" s="4">
         <v>4994</v>
       </c>
-      <c r="D10" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -948,11 +914,8 @@
       <c r="C11" s="4">
         <v>4994</v>
       </c>
-      <c r="D11" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -962,11 +925,8 @@
       <c r="C12" s="4">
         <v>4994</v>
       </c>
-      <c r="D12" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -976,11 +936,8 @@
       <c r="C13" s="4">
         <v>4994</v>
       </c>
-      <c r="D13" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -990,11 +947,8 @@
       <c r="C14" s="4">
         <v>4994</v>
       </c>
-      <c r="D14" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1004,11 +958,8 @@
       <c r="C15" s="4">
         <v>4994</v>
       </c>
-      <c r="D15" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1018,11 +969,8 @@
       <c r="C16" s="4">
         <v>4994</v>
       </c>
-      <c r="D16" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -1032,11 +980,8 @@
       <c r="C17" s="4">
         <v>4994</v>
       </c>
-      <c r="D17" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1046,11 +991,8 @@
       <c r="C18" s="4">
         <v>4994</v>
       </c>
-      <c r="D18" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1060,11 +1002,8 @@
       <c r="C19" s="4">
         <v>4994</v>
       </c>
-      <c r="D19" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -1074,11 +1013,8 @@
       <c r="C20" s="4">
         <v>4994</v>
       </c>
-      <c r="D20" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -1088,11 +1024,8 @@
       <c r="C21" s="4">
         <v>4994</v>
       </c>
-      <c r="D21" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -1102,11 +1035,8 @@
       <c r="C22" s="4">
         <v>4994</v>
       </c>
-      <c r="D22" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -1116,11 +1046,8 @@
       <c r="C23" s="4">
         <v>4994</v>
       </c>
-      <c r="D23" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -1130,11 +1057,8 @@
       <c r="C24" s="4">
         <v>4994</v>
       </c>
-      <c r="D24" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -1144,11 +1068,8 @@
       <c r="C25" s="4">
         <v>4994</v>
       </c>
-      <c r="D25" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
@@ -1158,11 +1079,8 @@
       <c r="C26" s="4">
         <v>4994</v>
       </c>
-      <c r="D26" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>52</v>
       </c>
@@ -1172,11 +1090,8 @@
       <c r="C27" s="4">
         <v>4994</v>
       </c>
-      <c r="D27" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>54</v>
       </c>
@@ -1186,11 +1101,8 @@
       <c r="C28" s="4">
         <v>4994</v>
       </c>
-      <c r="D28" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>56</v>
       </c>
@@ -1200,11 +1112,8 @@
       <c r="C29" s="4">
         <v>4994</v>
       </c>
-      <c r="D29" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
@@ -1214,11 +1123,8 @@
       <c r="C30" s="4">
         <v>4994</v>
       </c>
-      <c r="D30" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>60</v>
       </c>
@@ -1228,11 +1134,8 @@
       <c r="C31" s="4">
         <v>4994</v>
       </c>
-      <c r="D31" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>62</v>
       </c>
@@ -1242,11 +1145,8 @@
       <c r="C32" s="4">
         <v>3410</v>
       </c>
-      <c r="D32" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>64</v>
       </c>
@@ -1256,11 +1156,8 @@
       <c r="C33" s="4">
         <v>3410</v>
       </c>
-      <c r="D33" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>66</v>
       </c>
@@ -1270,11 +1167,8 @@
       <c r="C34" s="4">
         <v>3410</v>
       </c>
-      <c r="D34" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>68</v>
       </c>
@@ -1284,11 +1178,8 @@
       <c r="C35" s="4">
         <v>3410</v>
       </c>
-      <c r="D35" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>70</v>
       </c>
@@ -1298,11 +1189,8 @@
       <c r="C36" s="4">
         <v>3410</v>
       </c>
-      <c r="D36" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>72</v>
       </c>
@@ -1312,11 +1200,8 @@
       <c r="C37" s="4">
         <v>3410</v>
       </c>
-      <c r="D37" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>74</v>
       </c>
@@ -1326,11 +1211,8 @@
       <c r="C38" s="4">
         <v>3410</v>
       </c>
-      <c r="D38" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>76</v>
       </c>
@@ -1340,11 +1222,8 @@
       <c r="C39" s="4">
         <v>3410</v>
       </c>
-      <c r="D39" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>78</v>
       </c>
@@ -1354,11 +1233,8 @@
       <c r="C40" s="4">
         <v>3410</v>
       </c>
-      <c r="D40" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>80</v>
       </c>
@@ -1368,11 +1244,8 @@
       <c r="C41" s="4">
         <v>3410</v>
       </c>
-      <c r="D41" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>82</v>
       </c>
@@ -1382,11 +1255,8 @@
       <c r="C42" s="4">
         <v>3410</v>
       </c>
-      <c r="D42" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>84</v>
       </c>
@@ -1396,11 +1266,8 @@
       <c r="C43" s="4">
         <v>3410</v>
       </c>
-      <c r="D43" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>86</v>
       </c>
@@ -1410,11 +1277,8 @@
       <c r="C44" s="4">
         <v>3410</v>
       </c>
-      <c r="D44" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>88</v>
       </c>
@@ -1424,11 +1288,8 @@
       <c r="C45" s="4">
         <v>3410</v>
       </c>
-      <c r="D45" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>90</v>
       </c>
@@ -1438,11 +1299,8 @@
       <c r="C46" s="4">
         <v>3410</v>
       </c>
-      <c r="D46" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>92</v>
       </c>
@@ -1452,11 +1310,8 @@
       <c r="C47" s="4">
         <v>3410</v>
       </c>
-      <c r="D47" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>94</v>
       </c>
@@ -1466,11 +1321,8 @@
       <c r="C48" s="4">
         <v>3410</v>
       </c>
-      <c r="D48" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>96</v>
       </c>
@@ -1479,9 +1331,6 @@
       </c>
       <c r="C49" s="4">
         <v>3410</v>
-      </c>
-      <c r="D49" s="4">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>